<commit_message>
sửa lại phần quay thưởng
</commit_message>
<xml_diff>
--- a/DMS/Templates/Lucky_Number.xlsx
+++ b/DMS/Templates/Lucky_Number.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rang Dong\DMS.BE\DMS\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35B72F91-BF20-4DE3-827A-E27A87CAE25D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42B8E8E0-8B33-4601-83F4-47B7E54A5694}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LuckyNumber" sheetId="1" r:id="rId1"/>
+    <sheet name="Organization" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>STT</t>
   </si>
@@ -37,13 +38,34 @@
   </si>
   <si>
     <t xml:space="preserve">Giá trị </t>
+  </si>
+  <si>
+    <t>Mã đơn vị áp dụng</t>
+  </si>
+  <si>
+    <t>Mã</t>
+  </si>
+  <si>
+    <t>Tên</t>
+  </si>
+  <si>
+    <t>{{Organizations.Code}}</t>
+  </si>
+  <si>
+    <t>{{Organizations.Name}}</t>
+  </si>
+  <si>
+    <t>END</t>
+  </si>
+  <si>
+    <t>Vui lòng insert bản ghi vào trên lòng này</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,13 +99,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -115,7 +151,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -123,10 +159,23 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -411,21 +460,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="31" style="2" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="31" style="7" customWidth="1"/>
+    <col min="5" max="5" width="26.28515625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75">
+    <row r="1" spans="1:5" ht="18.75">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -437,6 +487,24 @@
       </c>
       <c r="D1" s="4" t="s">
         <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" ht="30">
+      <c r="A3" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -444,4 +512,40 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{302F3456-E799-4316-91E4-5E042F1ECC5E}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="2" max="2" width="39.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="18.75">
+      <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
DMS: Translate LuckyNumber Template
</commit_message>
<xml_diff>
--- a/DMS/Templates/Lucky_Number.xlsx
+++ b/DMS/Templates/Lucky_Number.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rang Dong\DMS.BE\DMS\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\dotNet\DMS\DMS.BE\DMS\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42B8E8E0-8B33-4601-83F4-47B7E54A5694}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C3EAB5-1022-4DE9-AC8C-CFEFBDFA38F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="LuckyNumber" sheetId="1" r:id="rId1"/>
-    <sheet name="Organization" sheetId="2" r:id="rId2"/>
+    <sheet name="Giải thưởng" sheetId="1" r:id="rId1"/>
+    <sheet name="Đơn vị tổ chức" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>

</xml_diff>